<commit_message>
Adds DataSetter and more code visual updates
</commit_message>
<xml_diff>
--- a/inicjaly.xlsx
+++ b/inicjaly.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -46,11 +45,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -129,10 +134,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -170,69 +175,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -256,54 +263,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -313,7 +319,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -322,7 +328,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -331,7 +337,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -339,10 +345,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -371,7 +377,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -384,13 +390,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -410,1731 +415,1741 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>First name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Last name</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="C1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Adam</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Czarnecki</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>A. C.</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Sadowska</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>B. S.</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Artur</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Woźniak</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>A. W.</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Barbara</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>Malinowska</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>B. M.</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Teresa</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Kołodziej</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>T. K.</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Maria</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Cieślak</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>M. C.</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Krystyna</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Kaczmarek</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>K. K.</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Laskowski</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>J. L.</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Edward</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>E. A.</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Józef</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>Sobczak</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>J. S.</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="12" ht="18.75" customHeight="1">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Justyna</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>Maciejewska</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>J. M.</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Mieczysław</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Kaźmierczak</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Marta</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>Kaźmierczak</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="15" ht="18.75" customHeight="1">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>Roman</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>Mazur</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>R. M.</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="16" ht="18.75" customHeight="1">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>Jasiński</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>Ł. J.</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="17" ht="18.75" customHeight="1">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Krzysztof</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>Kozłowski</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>K. K.</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>Laskowska</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>B. L.</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="19" ht="18.75" customHeight="1">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Józef</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>Wójcik</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>J. W.</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="20" ht="18.75" customHeight="1">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Zdzisław</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>Mazurek</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>Z. M.</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="21" ht="18.75" customHeight="1">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>Krzysztof</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>Borkowski</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>K. B.</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="22" ht="18.75" customHeight="1">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Zdzisław</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>Wasilewski</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="2" t="inlineStr">
         <is>
           <t>Z. W.</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="23" ht="18.75" customHeight="1">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>Wieczorek</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>J. W.</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="24" ht="18.75" customHeight="1">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>Artur</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>Szymański</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>A. S.</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="25" ht="18.75" customHeight="1">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>Kubiak</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>Ł. K.</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="26" ht="18.75" customHeight="1">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Danuta</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>Kowalczyk</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>D. K.</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="27" ht="18.75" customHeight="1">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Danuta</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>Walczak</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>D. W.</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="28" ht="18.75" customHeight="1">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Joanna</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>J. A.</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="29" ht="18.75" customHeight="1">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>Zdzisław</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="2" t="inlineStr">
         <is>
           <t>Wróbel</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="2" t="inlineStr">
         <is>
           <t>Z. W.</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="30" ht="18.75" customHeight="1">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>Baranowski</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="2" t="inlineStr">
         <is>
           <t>Ł. B.</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="31" ht="18.75" customHeight="1">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>Jerzy</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="2" t="inlineStr">
         <is>
           <t>J. A.</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+    <row r="32" ht="18.75" customHeight="1">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>Kołodziej</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="2" t="inlineStr">
         <is>
           <t>B. K.</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="33" ht="18.75" customHeight="1">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>Marianna</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
         <is>
           <t>Zawadzka</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="2" t="inlineStr">
         <is>
           <t>M. Z.</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
+    <row r="34" ht="18.75" customHeight="1">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>Karolina</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="2" t="inlineStr">
         <is>
           <t>Kaczmarek</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="2" t="inlineStr">
         <is>
           <t>K. K.</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="35" ht="18.75" customHeight="1">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>Czesław</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>Pietrzak</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="2" t="inlineStr">
         <is>
           <t>C. P.</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+    <row r="36" ht="18.75" customHeight="1">
+      <c r="A36" s="2" t="inlineStr">
         <is>
           <t>Mariusz</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="2" t="inlineStr">
         <is>
           <t>Zieliński</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="2" t="inlineStr">
         <is>
           <t>M. Z.</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+    <row r="37" ht="18.75" customHeight="1">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>Edward</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>Jakubowski</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="2" t="inlineStr">
         <is>
           <t>E. J.</t>
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+    <row r="38" ht="18.75" customHeight="1">
+      <c r="A38" s="2" t="inlineStr">
         <is>
           <t>Roman</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="2" t="inlineStr">
         <is>
           <t>Woźniak</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="2" t="inlineStr">
         <is>
           <t>R. W.</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+    <row r="39" ht="18.75" customHeight="1">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>Tadeusz</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>Nowakowski</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="2" t="inlineStr">
         <is>
           <t>T. N.</t>
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+    <row r="40" ht="18.75" customHeight="1">
+      <c r="A40" s="2" t="inlineStr">
         <is>
           <t>Marzena</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="2" t="inlineStr">
         <is>
           <t>Pawlak</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="2" t="inlineStr">
         <is>
           <t>M. P.</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="41" ht="18.75" customHeight="1">
+      <c r="A41" s="2" t="inlineStr">
         <is>
           <t>Agata</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="2" t="inlineStr">
         <is>
           <t>Kowalska</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="2" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+    <row r="42" ht="18.75" customHeight="1">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>Marcin</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="2" t="inlineStr">
         <is>
           <t>Lis</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="2" t="inlineStr">
         <is>
           <t>M. L.</t>
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+    <row r="43" ht="18.75" customHeight="1">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>Jadwiga</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>Ziółkowska</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="2" t="inlineStr">
         <is>
           <t>J. Z.</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="44" ht="18.75" customHeight="1">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>Sławomir</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>Jankowski</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="2" t="inlineStr">
         <is>
           <t>S. J.</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+    <row r="45" ht="18.75" customHeight="1">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>Teresa</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="2" t="inlineStr">
         <is>
           <t>Piotrowska</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="2" t="inlineStr">
         <is>
           <t>T. P.</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="46" ht="18.75" customHeight="1">
+      <c r="A46" s="2" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="2" t="inlineStr">
         <is>
           <t>Przybylski</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="2" t="inlineStr">
         <is>
           <t>P. P.</t>
         </is>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
+    <row r="47" ht="18.75" customHeight="1">
+      <c r="A47" s="2" t="inlineStr">
         <is>
           <t>Ryszard</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="2" t="inlineStr">
         <is>
           <t>Nowicki</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="2" t="inlineStr">
         <is>
           <t>R. N.</t>
         </is>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+    <row r="48" ht="18.75" customHeight="1">
+      <c r="A48" s="2" t="inlineStr">
         <is>
           <t>Marcin</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="2" t="inlineStr">
         <is>
           <t>Borkowski</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="2" t="inlineStr">
         <is>
           <t>M. B.</t>
         </is>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
+    <row r="49" ht="18.75" customHeight="1">
+      <c r="A49" s="2" t="inlineStr">
         <is>
           <t>Sylwia</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="2" t="inlineStr">
         <is>
           <t>Gajewska</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="2" t="inlineStr">
         <is>
           <t>S. G.</t>
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+    <row r="50" ht="18.75" customHeight="1">
+      <c r="A50" s="2" t="inlineStr">
         <is>
           <t>Tadeusz</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="2" t="inlineStr">
         <is>
           <t>Malinowski</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="2" t="inlineStr">
         <is>
           <t>T. M.</t>
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
+    <row r="51" ht="18.75" customHeight="1">
+      <c r="A51" s="2" t="inlineStr">
         <is>
           <t>Marta</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="2" t="inlineStr">
         <is>
           <t>Wieczorek</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="2" t="inlineStr">
         <is>
           <t>M. W.</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+    <row r="52" ht="18.75" customHeight="1">
+      <c r="A52" s="2" t="inlineStr">
         <is>
           <t>Kamil</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B52" s="2" t="inlineStr">
         <is>
           <t>Pawłowski</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C52" s="2" t="inlineStr">
         <is>
           <t>K. P.</t>
         </is>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+    <row r="53" ht="18.75" customHeight="1">
+      <c r="A53" s="2" t="inlineStr">
         <is>
           <t>Halina</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B53" s="2" t="inlineStr">
         <is>
           <t>Urbańska</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C53" s="2" t="inlineStr">
         <is>
           <t>H. U.</t>
         </is>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+    <row r="54" ht="18.75" customHeight="1">
+      <c r="A54" s="2" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B54" s="2" t="inlineStr">
         <is>
           <t>Pietrzak</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C54" s="2" t="inlineStr">
         <is>
           <t>B. P.</t>
         </is>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+    <row r="55" ht="18.75" customHeight="1">
+      <c r="A55" s="2" t="inlineStr">
         <is>
           <t>Marianna</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="2" t="inlineStr">
         <is>
           <t>Wójcik</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C55" s="2" t="inlineStr">
         <is>
           <t>M. W.</t>
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+    <row r="56" ht="18.75" customHeight="1">
+      <c r="A56" s="2" t="inlineStr">
         <is>
           <t>Ewelina</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B56" s="2" t="inlineStr">
         <is>
           <t>Górska</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C56" s="2" t="inlineStr">
         <is>
           <t>E. G.</t>
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
+    <row r="57" ht="18.75" customHeight="1">
+      <c r="A57" s="2" t="inlineStr">
         <is>
           <t>Krzysztof</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B57" s="2" t="inlineStr">
         <is>
           <t>Michalak</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C57" s="2" t="inlineStr">
         <is>
           <t>K. M.</t>
         </is>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
+    <row r="58" ht="18.75" customHeight="1">
+      <c r="A58" s="2" t="inlineStr">
         <is>
           <t>Ewa</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B58" s="2" t="inlineStr">
         <is>
           <t>Dąbrowska</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C58" s="2" t="inlineStr">
         <is>
           <t>E. D.</t>
         </is>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
+    <row r="59" ht="18.75" customHeight="1">
+      <c r="A59" s="2" t="inlineStr">
         <is>
           <t>Andrzej</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B59" s="2" t="inlineStr">
         <is>
           <t>Wieczorek</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="C59" s="2" t="inlineStr">
         <is>
           <t>A. W.</t>
         </is>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
+    <row r="60" ht="18.75" customHeight="1">
+      <c r="A60" s="2" t="inlineStr">
         <is>
           <t>Elżbieta</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B60" s="2" t="inlineStr">
         <is>
           <t>Wiśniewska</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C60" s="2" t="inlineStr">
         <is>
           <t>E. W.</t>
         </is>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
+    <row r="61" ht="18.75" customHeight="1">
+      <c r="A61" s="2" t="inlineStr">
         <is>
           <t>Grażyna</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B61" s="2" t="inlineStr">
         <is>
           <t>Zakrzewska</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C61" s="2" t="inlineStr">
         <is>
           <t>G. Z.</t>
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+    <row r="62" ht="18.75" customHeight="1">
+      <c r="A62" s="2" t="inlineStr">
         <is>
           <t>Monika</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B62" s="2" t="inlineStr">
         <is>
           <t>Kamińska</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C62" s="2" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
+    <row r="63" ht="18.75" customHeight="1">
+      <c r="A63" s="2" t="inlineStr">
         <is>
           <t>Alicja</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B63" s="2" t="inlineStr">
         <is>
           <t>Kozłowska</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C63" s="2" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
+    <row r="64" ht="18.75" customHeight="1">
+      <c r="A64" s="2" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B64" s="2" t="inlineStr">
         <is>
           <t>Nowakowski</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="C64" s="2" t="inlineStr">
         <is>
           <t>P. N.</t>
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
+    <row r="65" ht="18.75" customHeight="1">
+      <c r="A65" s="2" t="inlineStr">
         <is>
           <t>Katarzyna</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B65" s="2" t="inlineStr">
         <is>
           <t>Gajewska</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C65" s="2" t="inlineStr">
         <is>
           <t>K. G.</t>
         </is>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
+    <row r="66" ht="18.75" customHeight="1">
+      <c r="A66" s="2" t="inlineStr">
         <is>
           <t>Agata</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B66" s="2" t="inlineStr">
         <is>
           <t>Pietrzak</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C66" s="2" t="inlineStr">
         <is>
           <t>A. P.</t>
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
+    <row r="67" ht="18.75" customHeight="1">
+      <c r="A67" s="2" t="inlineStr">
         <is>
           <t>Edward</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B67" s="2" t="inlineStr">
         <is>
           <t>Jankowski</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C67" s="2" t="inlineStr">
         <is>
           <t>E. J.</t>
         </is>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
+    <row r="68" ht="18.75" customHeight="1">
+      <c r="A68" s="2" t="inlineStr">
         <is>
           <t>Jakub</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B68" s="2" t="inlineStr">
         <is>
           <t>Krajewski</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C68" s="2" t="inlineStr">
         <is>
           <t>J. K.</t>
         </is>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
+    <row r="69" ht="18.75" customHeight="1">
+      <c r="A69" s="2" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B69" s="2" t="inlineStr">
         <is>
           <t>Szulc</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C69" s="2" t="inlineStr">
         <is>
           <t>J. S.</t>
         </is>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="70" ht="18.75" customHeight="1">
+      <c r="A70" s="2" t="inlineStr">
         <is>
           <t>Alicja</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B70" s="2" t="inlineStr">
         <is>
           <t>Krajewska</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C70" s="2" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
+    <row r="71" ht="18.75" customHeight="1">
+      <c r="A71" s="2" t="inlineStr">
         <is>
           <t>Stefania</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B71" s="2" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C71" s="2" t="inlineStr">
         <is>
           <t>S. A.</t>
         </is>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
+    <row r="72" ht="18.75" customHeight="1">
+      <c r="A72" s="2" t="inlineStr">
         <is>
           <t>Daniel</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B72" s="2" t="inlineStr">
         <is>
           <t>Majewski</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C72" s="2" t="inlineStr">
         <is>
           <t>D. M.</t>
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
+    <row r="73" ht="18.75" customHeight="1">
+      <c r="A73" s="2" t="inlineStr">
         <is>
           <t>Leszek</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B73" s="2" t="inlineStr">
         <is>
           <t>Wasilewski</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C73" s="2" t="inlineStr">
         <is>
           <t>L. W.</t>
         </is>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
+    <row r="74" ht="18.75" customHeight="1">
+      <c r="A74" s="2" t="inlineStr">
         <is>
           <t>Maria</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B74" s="2" t="inlineStr">
         <is>
           <t>Kucharska</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C74" s="2" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
+    <row r="75" ht="18.75" customHeight="1">
+      <c r="A75" s="2" t="inlineStr">
         <is>
           <t>Dawid</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B75" s="2" t="inlineStr">
         <is>
           <t>Szulc</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C75" s="2" t="inlineStr">
         <is>
           <t>D. S.</t>
         </is>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
+    <row r="76" ht="18.75" customHeight="1">
+      <c r="A76" s="2" t="inlineStr">
         <is>
           <t>Sławomir</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B76" s="2" t="inlineStr">
         <is>
           <t>Zając</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C76" s="2" t="inlineStr">
         <is>
           <t>S. Z.</t>
         </is>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
+    <row r="77" ht="18.75" customHeight="1">
+      <c r="A77" s="2" t="inlineStr">
         <is>
           <t>Monika</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B77" s="2" t="inlineStr">
         <is>
           <t>Nowakowska</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C77" s="2" t="inlineStr">
         <is>
           <t>M. N.</t>
         </is>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
+    <row r="78" ht="18.75" customHeight="1">
+      <c r="A78" s="2" t="inlineStr">
         <is>
           <t>Leszek</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B78" s="2" t="inlineStr">
         <is>
           <t>Brzeziński</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C78" s="2" t="inlineStr">
         <is>
           <t>L. B.</t>
         </is>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
+    <row r="79" ht="18.75" customHeight="1">
+      <c r="A79" s="2" t="inlineStr">
         <is>
           <t>Jarosław</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B79" s="2" t="inlineStr">
         <is>
           <t>Majewski</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C79" s="2" t="inlineStr">
         <is>
           <t>J. M.</t>
         </is>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
+    <row r="80" ht="18.75" customHeight="1">
+      <c r="A80" s="2" t="inlineStr">
         <is>
           <t>Mariusz</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="B80" s="2" t="inlineStr">
         <is>
           <t>Majewski</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="C80" s="2" t="inlineStr">
         <is>
           <t>M. M.</t>
         </is>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
+    <row r="81" ht="18.75" customHeight="1">
+      <c r="A81" s="2" t="inlineStr">
         <is>
           <t>Stanisław</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B81" s="2" t="inlineStr">
         <is>
           <t>Baran</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C81" s="2" t="inlineStr">
         <is>
           <t>S. B.</t>
         </is>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
+    <row r="82" ht="18.75" customHeight="1">
+      <c r="A82" s="2" t="inlineStr">
         <is>
           <t>Andrzej</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B82" s="2" t="inlineStr">
         <is>
           <t>Dąbrowski</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="C82" s="2" t="inlineStr">
         <is>
           <t>A. D.</t>
         </is>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
+    <row r="83" ht="18.75" customHeight="1">
+      <c r="A83" s="2" t="inlineStr">
         <is>
           <t>Dawid</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B83" s="2" t="inlineStr">
         <is>
           <t>Sobczak</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="C83" s="2" t="inlineStr">
         <is>
           <t>D. S.</t>
         </is>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
+    <row r="84" ht="18.75" customHeight="1">
+      <c r="A84" s="2" t="inlineStr">
         <is>
           <t>Magdalena</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B84" s="2" t="inlineStr">
         <is>
           <t>Lis</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C84" s="2" t="inlineStr">
         <is>
           <t>M. L.</t>
         </is>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
+    <row r="85" ht="18.75" customHeight="1">
+      <c r="A85" s="2" t="inlineStr">
         <is>
           <t>Karolina</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B85" s="2" t="inlineStr">
         <is>
           <t>Zając</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="C85" s="2" t="inlineStr">
         <is>
           <t>K. Z.</t>
         </is>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
+    <row r="86" ht="18.75" customHeight="1">
+      <c r="A86" s="2" t="inlineStr">
         <is>
           <t>Adam</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B86" s="2" t="inlineStr">
         <is>
           <t>Kaczmarek</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C86" s="2" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
+    <row r="87" ht="18.75" customHeight="1">
+      <c r="A87" s="2" t="inlineStr">
         <is>
           <t>Czesław</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B87" s="2" t="inlineStr">
         <is>
           <t>Kowalczyk</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C87" s="2" t="inlineStr">
         <is>
           <t>C. K.</t>
         </is>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
+    <row r="88" ht="18.75" customHeight="1">
+      <c r="A88" s="2" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B88" s="2" t="inlineStr">
         <is>
           <t>Jaworski</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="C88" s="2" t="inlineStr">
         <is>
           <t>Ł. J.</t>
         </is>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
+    <row r="89" ht="18.75" customHeight="1">
+      <c r="A89" s="2" t="inlineStr">
         <is>
           <t>Marta</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B89" s="2" t="inlineStr">
         <is>
           <t>Jakubowska</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="C89" s="2" t="inlineStr">
         <is>
           <t>M. J.</t>
         </is>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
+    <row r="90" ht="18.75" customHeight="1">
+      <c r="A90" s="2" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B90" s="2" t="inlineStr">
         <is>
           <t>Woźniak</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="C90" s="2" t="inlineStr">
         <is>
           <t>P. W.</t>
         </is>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
+    <row r="91" ht="18.75" customHeight="1">
+      <c r="A91" s="2" t="inlineStr">
         <is>
           <t>Monika</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="B91" s="2" t="inlineStr">
         <is>
           <t>Zając</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="C91" s="2" t="inlineStr">
         <is>
           <t>M. Z.</t>
         </is>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
+    <row r="92" ht="18.75" customHeight="1">
+      <c r="A92" s="2" t="inlineStr">
         <is>
           <t>Waldemar</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
+      <c r="B92" s="2" t="inlineStr">
         <is>
           <t>Witkowski</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="C92" s="2" t="inlineStr">
         <is>
           <t>W. W.</t>
         </is>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
+    <row r="93" ht="18.75" customHeight="1">
+      <c r="A93" s="2" t="inlineStr">
         <is>
           <t>Izabela</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="B93" s="2" t="inlineStr">
         <is>
           <t>Król</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
+      <c r="C93" s="2" t="inlineStr">
         <is>
           <t>I. K.</t>
         </is>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
+    <row r="94" ht="18.75" customHeight="1">
+      <c r="A94" s="2" t="inlineStr">
         <is>
           <t>Mateusz</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="B94" s="2" t="inlineStr">
         <is>
           <t>Przybylski</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
+      <c r="C94" s="2" t="inlineStr">
         <is>
           <t>M. P.</t>
         </is>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
+    <row r="95" ht="18.75" customHeight="1">
+      <c r="A95" s="2" t="inlineStr">
         <is>
           <t>Stanisław</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="B95" s="2" t="inlineStr">
         <is>
           <t>Jasiński</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="C95" s="2" t="inlineStr">
         <is>
           <t>S. J.</t>
         </is>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
+    <row r="96" ht="18.75" customHeight="1">
+      <c r="A96" s="2" t="inlineStr">
         <is>
           <t>Wiesława</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
+      <c r="B96" s="2" t="inlineStr">
         <is>
           <t>Adamska</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="C96" s="2" t="inlineStr">
         <is>
           <t>W. A.</t>
         </is>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
+    <row r="97" ht="18.75" customHeight="1">
+      <c r="A97" s="2" t="inlineStr">
         <is>
           <t>Helena</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
+      <c r="B97" s="2" t="inlineStr">
         <is>
           <t>Jabłońska</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
+      <c r="C97" s="2" t="inlineStr">
         <is>
           <t>H. J.</t>
         </is>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
+    <row r="98" ht="18.75" customHeight="1">
+      <c r="A98" s="2" t="inlineStr">
         <is>
           <t>Irena</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
+      <c r="B98" s="2" t="inlineStr">
         <is>
           <t>Zielińska</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="C98" s="2" t="inlineStr">
         <is>
           <t>I. Z.</t>
         </is>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
+    <row r="99" ht="18.75" customHeight="1">
+      <c r="A99" s="2" t="inlineStr">
         <is>
           <t>Halina</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B99" s="2" t="inlineStr">
         <is>
           <t>Przybylska</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
+      <c r="C99" s="2" t="inlineStr">
         <is>
           <t>H. P.</t>
         </is>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
+    <row r="100" ht="18.75" customHeight="1">
+      <c r="A100" s="2" t="inlineStr">
         <is>
           <t>Izabela</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
+      <c r="B100" s="2" t="inlineStr">
         <is>
           <t>Czarnecka</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="C100" s="2" t="inlineStr">
         <is>
           <t>I. C.</t>
         </is>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
+    <row r="101" ht="18.75" customHeight="1">
+      <c r="A101" s="2" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
+      <c r="B101" s="2" t="inlineStr">
         <is>
           <t>Chmielewski</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="C101" s="2" t="inlineStr">
         <is>
           <t>P. C.</t>
         </is>
       </c>
     </row>
-    <row r="102"/>
+    <row r="102" ht="18.75" customHeight="1">
+      <c r="A102" s="2" t="n"/>
+      <c r="B102" s="2" t="n"/>
+      <c r="C102" s="2" t="n"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Heh I did some progress
</commit_message>
<xml_diff>
--- a/inicjaly.xlsx
+++ b/inicjaly.xlsx
@@ -16,13 +16,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -33,7 +39,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -43,15 +56,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,7 +443,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,1728 +451,2360 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="16.29071428571428" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>First name</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Last name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="n"/>
-    </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="C1" s="5" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="5" t="n"/>
+      <c r="G1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>Adam</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>Czarnecki</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>A. C.</t>
         </is>
       </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>Wylosowane imie</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Wygrana kwota</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="n"/>
+      <c r="G2" s="2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>Sadowska</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>B. S.</t>
         </is>
       </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="5" t="n"/>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Artur</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>Woźniak</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>A. W.</t>
         </is>
       </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Piotr</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="F4" s="5" t="n"/>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>Barbara</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Malinowska</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>B. M.</t>
         </is>
       </c>
-    </row>
-    <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" s="5" t="n"/>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Teresa</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Kołodziej</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>T. K.</t>
         </is>
       </c>
-    </row>
-    <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="5" t="n"/>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>Maria</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>Cieślak</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>M. C.</t>
         </is>
       </c>
-    </row>
-    <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="5" t="n"/>
+      <c r="G7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="19.5" customHeight="1">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>Krystyna</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>Kaczmarek</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>K. K.</t>
         </is>
       </c>
-    </row>
-    <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="5" t="n"/>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" ht="19.5" customHeight="1">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Laskowski</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>J. L.</t>
         </is>
       </c>
-    </row>
-    <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="5" t="n"/>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="19.5" customHeight="1">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>Edward</t>
         </is>
       </c>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>E. A.</t>
         </is>
       </c>
-    </row>
-    <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="5" t="n"/>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" ht="19.5" customHeight="1">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>Józef</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>Sobczak</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>J. S.</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" s="5" t="n"/>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="19.5" customHeight="1">
+      <c r="A12" s="5" t="inlineStr">
         <is>
           <t>Justyna</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="B12" s="5" t="inlineStr">
         <is>
           <t>Maciejewska</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>J. M.</t>
         </is>
       </c>
-    </row>
-    <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="5" t="n"/>
+      <c r="G12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" ht="19.5" customHeight="1">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>Mieczysław</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" s="5" t="inlineStr">
         <is>
           <t>Kaźmierczak</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="5" t="n"/>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" s="5" t="inlineStr">
         <is>
           <t>Marta</t>
         </is>
       </c>
-      <c r="B14" s="2" t="inlineStr">
+      <c r="B14" s="5" t="inlineStr">
         <is>
           <t>Kaźmierczak</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="C14" s="3" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="5" t="n"/>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="A15" s="5" t="inlineStr">
         <is>
           <t>Roman</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B15" s="5" t="inlineStr">
         <is>
           <t>Mazur</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C15" s="3" t="inlineStr">
         <is>
           <t>R. M.</t>
         </is>
       </c>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="5" t="n"/>
+      <c r="G15" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B16" s="2" t="inlineStr">
+      <c r="B16" s="5" t="inlineStr">
         <is>
           <t>Jasiński</t>
         </is>
       </c>
-      <c r="C16" s="2" t="inlineStr">
+      <c r="C16" s="3" t="inlineStr">
         <is>
           <t>Ł. J.</t>
         </is>
       </c>
+      <c r="D16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
+      <c r="F16" s="5" t="n"/>
+      <c r="G16" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" ht="18.75" customHeight="1">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
         <is>
           <t>Krzysztof</t>
         </is>
       </c>
-      <c r="B17" s="2" t="inlineStr">
+      <c r="B17" s="5" t="inlineStr">
         <is>
           <t>Kozłowski</t>
         </is>
       </c>
-      <c r="C17" s="2" t="inlineStr">
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>K. K.</t>
         </is>
       </c>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="5" t="n"/>
+      <c r="G17" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="2" t="inlineStr">
+      <c r="A18" s="5" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B18" s="2" t="inlineStr">
+      <c r="B18" s="5" t="inlineStr">
         <is>
           <t>Laskowska</t>
         </is>
       </c>
-      <c r="C18" s="2" t="inlineStr">
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>B. L.</t>
         </is>
       </c>
+      <c r="D18" s="2" t="n"/>
+      <c r="E18" s="2" t="n"/>
+      <c r="F18" s="5" t="n"/>
+      <c r="G18" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="2" t="inlineStr">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>Józef</t>
         </is>
       </c>
-      <c r="B19" s="2" t="inlineStr">
+      <c r="B19" s="5" t="inlineStr">
         <is>
           <t>Wójcik</t>
         </is>
       </c>
-      <c r="C19" s="2" t="inlineStr">
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>J. W.</t>
         </is>
       </c>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="5" t="n"/>
+      <c r="G19" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="2" t="inlineStr">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>Zdzisław</t>
         </is>
       </c>
-      <c r="B20" s="2" t="inlineStr">
+      <c r="B20" s="5" t="inlineStr">
         <is>
           <t>Mazurek</t>
         </is>
       </c>
-      <c r="C20" s="2" t="inlineStr">
+      <c r="C20" s="3" t="inlineStr">
         <is>
           <t>Z. M.</t>
         </is>
       </c>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="5" t="n"/>
+      <c r="G20" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" ht="18.75" customHeight="1">
-      <c r="A21" s="2" t="inlineStr">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>Krzysztof</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
+      <c r="B21" s="5" t="inlineStr">
         <is>
           <t>Borkowski</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t>K. B.</t>
         </is>
       </c>
+      <c r="D21" s="2" t="n"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="5" t="n"/>
+      <c r="G21" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="2" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>Zdzisław</t>
         </is>
       </c>
-      <c r="B22" s="2" t="inlineStr">
+      <c r="B22" s="5" t="inlineStr">
         <is>
           <t>Wasilewski</t>
         </is>
       </c>
-      <c r="C22" s="2" t="inlineStr">
+      <c r="C22" s="3" t="inlineStr">
         <is>
           <t>Z. W.</t>
         </is>
       </c>
+      <c r="D22" s="2" t="n"/>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="5" t="n"/>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" ht="18.75" customHeight="1">
-      <c r="A23" s="2" t="inlineStr">
+      <c r="A23" s="5" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B23" s="5" t="inlineStr">
         <is>
           <t>Wieczorek</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr">
+      <c r="C23" s="3" t="inlineStr">
         <is>
           <t>J. W.</t>
         </is>
       </c>
+      <c r="D23" s="2" t="n"/>
+      <c r="E23" s="2" t="n"/>
+      <c r="F23" s="5" t="n"/>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" ht="18.75" customHeight="1">
-      <c r="A24" s="2" t="inlineStr">
+      <c r="A24" s="5" t="inlineStr">
         <is>
           <t>Artur</t>
         </is>
       </c>
-      <c r="B24" s="2" t="inlineStr">
+      <c r="B24" s="5" t="inlineStr">
         <is>
           <t>Szymański</t>
         </is>
       </c>
-      <c r="C24" s="2" t="inlineStr">
+      <c r="C24" s="3" t="inlineStr">
         <is>
           <t>A. S.</t>
         </is>
       </c>
-    </row>
-    <row r="25" ht="18.75" customHeight="1">
-      <c r="A25" s="2" t="inlineStr">
+      <c r="D24" s="2" t="n"/>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="5" t="n"/>
+      <c r="G24" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" ht="19.5" customHeight="1">
+      <c r="A25" s="5" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B25" s="2" t="inlineStr">
+      <c r="B25" s="5" t="inlineStr">
         <is>
           <t>Kubiak</t>
         </is>
       </c>
-      <c r="C25" s="2" t="inlineStr">
+      <c r="C25" s="3" t="inlineStr">
         <is>
           <t>Ł. K.</t>
         </is>
       </c>
-    </row>
-    <row r="26" ht="18.75" customHeight="1">
-      <c r="A26" s="2" t="inlineStr">
+      <c r="D25" s="2" t="n"/>
+      <c r="E25" s="2" t="n"/>
+      <c r="F25" s="5" t="n"/>
+      <c r="G25" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="19.5" customHeight="1">
+      <c r="A26" s="5" t="inlineStr">
         <is>
           <t>Danuta</t>
         </is>
       </c>
-      <c r="B26" s="2" t="inlineStr">
+      <c r="B26" s="5" t="inlineStr">
         <is>
           <t>Kowalczyk</t>
         </is>
       </c>
-      <c r="C26" s="2" t="inlineStr">
+      <c r="C26" s="3" t="inlineStr">
         <is>
           <t>D. K.</t>
         </is>
       </c>
-    </row>
-    <row r="27" ht="18.75" customHeight="1">
-      <c r="A27" s="2" t="inlineStr">
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
+      <c r="F26" s="5" t="n"/>
+      <c r="G26" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="19.5" customHeight="1">
+      <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Danuta</t>
         </is>
       </c>
-      <c r="B27" s="2" t="inlineStr">
+      <c r="B27" s="5" t="inlineStr">
         <is>
           <t>Walczak</t>
         </is>
       </c>
-      <c r="C27" s="2" t="inlineStr">
+      <c r="C27" s="3" t="inlineStr">
         <is>
           <t>D. W.</t>
         </is>
       </c>
-    </row>
-    <row r="28" ht="18.75" customHeight="1">
-      <c r="A28" s="2" t="inlineStr">
+      <c r="D27" s="2" t="n"/>
+      <c r="E27" s="2" t="n"/>
+      <c r="F27" s="5" t="n"/>
+      <c r="G27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="19.5" customHeight="1">
+      <c r="A28" s="5" t="inlineStr">
         <is>
           <t>Joanna</t>
         </is>
       </c>
-      <c r="B28" s="2" t="inlineStr">
+      <c r="B28" s="5" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C28" s="2" t="inlineStr">
+      <c r="C28" s="3" t="inlineStr">
         <is>
           <t>J. A.</t>
         </is>
       </c>
-    </row>
-    <row r="29" ht="18.75" customHeight="1">
-      <c r="A29" s="2" t="inlineStr">
+      <c r="D28" s="2" t="n"/>
+      <c r="E28" s="2" t="n"/>
+      <c r="F28" s="5" t="n"/>
+      <c r="G28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="19.5" customHeight="1">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>Zdzisław</t>
         </is>
       </c>
-      <c r="B29" s="2" t="inlineStr">
+      <c r="B29" s="5" t="inlineStr">
         <is>
           <t>Wróbel</t>
         </is>
       </c>
-      <c r="C29" s="2" t="inlineStr">
+      <c r="C29" s="3" t="inlineStr">
         <is>
           <t>Z. W.</t>
         </is>
       </c>
-    </row>
-    <row r="30" ht="18.75" customHeight="1">
-      <c r="A30" s="2" t="inlineStr">
+      <c r="D29" s="2" t="n"/>
+      <c r="E29" s="2" t="n"/>
+      <c r="F29" s="5" t="n"/>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="19.5" customHeight="1">
+      <c r="A30" s="5" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B30" s="2" t="inlineStr">
+      <c r="B30" s="5" t="inlineStr">
         <is>
           <t>Baranowski</t>
         </is>
       </c>
-      <c r="C30" s="2" t="inlineStr">
+      <c r="C30" s="3" t="inlineStr">
         <is>
           <t>Ł. B.</t>
         </is>
       </c>
-    </row>
-    <row r="31" ht="18.75" customHeight="1">
-      <c r="A31" s="2" t="inlineStr">
+      <c r="D30" s="2" t="n"/>
+      <c r="E30" s="2" t="n"/>
+      <c r="F30" s="5" t="n"/>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="19.5" customHeight="1">
+      <c r="A31" s="5" t="inlineStr">
         <is>
           <t>Jerzy</t>
         </is>
       </c>
-      <c r="B31" s="2" t="inlineStr">
+      <c r="B31" s="5" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C31" s="2" t="inlineStr">
+      <c r="C31" s="3" t="inlineStr">
         <is>
           <t>J. A.</t>
         </is>
       </c>
-    </row>
-    <row r="32" ht="18.75" customHeight="1">
-      <c r="A32" s="2" t="inlineStr">
+      <c r="D31" s="2" t="n"/>
+      <c r="E31" s="2" t="n"/>
+      <c r="F31" s="5" t="n"/>
+      <c r="G31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="19.5" customHeight="1">
+      <c r="A32" s="5" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B32" s="2" t="inlineStr">
+      <c r="B32" s="5" t="inlineStr">
         <is>
           <t>Kołodziej</t>
         </is>
       </c>
-      <c r="C32" s="2" t="inlineStr">
+      <c r="C32" s="3" t="inlineStr">
         <is>
           <t>B. K.</t>
         </is>
       </c>
-    </row>
-    <row r="33" ht="18.75" customHeight="1">
-      <c r="A33" s="2" t="inlineStr">
+      <c r="D32" s="2" t="n"/>
+      <c r="E32" s="2" t="n"/>
+      <c r="F32" s="5" t="n"/>
+      <c r="G32" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" ht="19.5" customHeight="1">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t>Marianna</t>
         </is>
       </c>
-      <c r="B33" s="2" t="inlineStr">
+      <c r="B33" s="5" t="inlineStr">
         <is>
           <t>Zawadzka</t>
         </is>
       </c>
-      <c r="C33" s="2" t="inlineStr">
+      <c r="C33" s="3" t="inlineStr">
         <is>
           <t>M. Z.</t>
         </is>
       </c>
-    </row>
-    <row r="34" ht="18.75" customHeight="1">
-      <c r="A34" s="2" t="inlineStr">
+      <c r="D33" s="2" t="n"/>
+      <c r="E33" s="2" t="n"/>
+      <c r="F33" s="5" t="n"/>
+      <c r="G33" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" ht="19.5" customHeight="1">
+      <c r="A34" s="5" t="inlineStr">
         <is>
           <t>Karolina</t>
         </is>
       </c>
-      <c r="B34" s="2" t="inlineStr">
+      <c r="B34" s="5" t="inlineStr">
         <is>
           <t>Kaczmarek</t>
         </is>
       </c>
-      <c r="C34" s="2" t="inlineStr">
+      <c r="C34" s="3" t="inlineStr">
         <is>
           <t>K. K.</t>
         </is>
       </c>
-    </row>
-    <row r="35" ht="18.75" customHeight="1">
-      <c r="A35" s="2" t="inlineStr">
+      <c r="D34" s="2" t="n"/>
+      <c r="E34" s="2" t="n"/>
+      <c r="F34" s="5" t="n"/>
+      <c r="G34" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" ht="19.5" customHeight="1">
+      <c r="A35" s="5" t="inlineStr">
         <is>
           <t>Czesław</t>
         </is>
       </c>
-      <c r="B35" s="2" t="inlineStr">
+      <c r="B35" s="5" t="inlineStr">
         <is>
           <t>Pietrzak</t>
         </is>
       </c>
-      <c r="C35" s="2" t="inlineStr">
+      <c r="C35" s="3" t="inlineStr">
         <is>
           <t>C. P.</t>
         </is>
       </c>
-    </row>
-    <row r="36" ht="18.75" customHeight="1">
-      <c r="A36" s="2" t="inlineStr">
+      <c r="D35" s="2" t="n"/>
+      <c r="E35" s="2" t="n"/>
+      <c r="F35" s="5" t="n"/>
+      <c r="G35" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" ht="19.5" customHeight="1">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>Mariusz</t>
         </is>
       </c>
-      <c r="B36" s="2" t="inlineStr">
+      <c r="B36" s="5" t="inlineStr">
         <is>
           <t>Zieliński</t>
         </is>
       </c>
-      <c r="C36" s="2" t="inlineStr">
+      <c r="C36" s="3" t="inlineStr">
         <is>
           <t>M. Z.</t>
         </is>
       </c>
-    </row>
-    <row r="37" ht="18.75" customHeight="1">
-      <c r="A37" s="2" t="inlineStr">
+      <c r="D36" s="2" t="n"/>
+      <c r="E36" s="2" t="n"/>
+      <c r="F36" s="5" t="n"/>
+      <c r="G36" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" ht="19.5" customHeight="1">
+      <c r="A37" s="5" t="inlineStr">
         <is>
           <t>Edward</t>
         </is>
       </c>
-      <c r="B37" s="2" t="inlineStr">
+      <c r="B37" s="5" t="inlineStr">
         <is>
           <t>Jakubowski</t>
         </is>
       </c>
-      <c r="C37" s="2" t="inlineStr">
+      <c r="C37" s="3" t="inlineStr">
         <is>
           <t>E. J.</t>
         </is>
       </c>
+      <c r="D37" s="2" t="n"/>
+      <c r="E37" s="2" t="n"/>
+      <c r="F37" s="5" t="n"/>
+      <c r="G37" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" ht="18.75" customHeight="1">
-      <c r="A38" s="2" t="inlineStr">
+      <c r="A38" s="5" t="inlineStr">
         <is>
           <t>Roman</t>
         </is>
       </c>
-      <c r="B38" s="2" t="inlineStr">
+      <c r="B38" s="5" t="inlineStr">
         <is>
           <t>Woźniak</t>
         </is>
       </c>
-      <c r="C38" s="2" t="inlineStr">
+      <c r="C38" s="3" t="inlineStr">
         <is>
           <t>R. W.</t>
         </is>
       </c>
+      <c r="D38" s="2" t="n"/>
+      <c r="E38" s="2" t="n"/>
+      <c r="F38" s="5" t="n"/>
+      <c r="G38" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" ht="18.75" customHeight="1">
-      <c r="A39" s="2" t="inlineStr">
+      <c r="A39" s="5" t="inlineStr">
         <is>
           <t>Tadeusz</t>
         </is>
       </c>
-      <c r="B39" s="2" t="inlineStr">
+      <c r="B39" s="5" t="inlineStr">
         <is>
           <t>Nowakowski</t>
         </is>
       </c>
-      <c r="C39" s="2" t="inlineStr">
+      <c r="C39" s="3" t="inlineStr">
         <is>
           <t>T. N.</t>
         </is>
       </c>
+      <c r="D39" s="2" t="n"/>
+      <c r="E39" s="2" t="n"/>
+      <c r="F39" s="5" t="n"/>
+      <c r="G39" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" ht="18.75" customHeight="1">
-      <c r="A40" s="2" t="inlineStr">
+      <c r="A40" s="5" t="inlineStr">
         <is>
           <t>Marzena</t>
         </is>
       </c>
-      <c r="B40" s="2" t="inlineStr">
+      <c r="B40" s="5" t="inlineStr">
         <is>
           <t>Pawlak</t>
         </is>
       </c>
-      <c r="C40" s="2" t="inlineStr">
+      <c r="C40" s="3" t="inlineStr">
         <is>
           <t>M. P.</t>
         </is>
       </c>
+      <c r="D40" s="2" t="n"/>
+      <c r="E40" s="2" t="n"/>
+      <c r="F40" s="5" t="n"/>
+      <c r="G40" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" ht="18.75" customHeight="1">
-      <c r="A41" s="2" t="inlineStr">
+      <c r="A41" s="5" t="inlineStr">
         <is>
           <t>Agata</t>
         </is>
       </c>
-      <c r="B41" s="2" t="inlineStr">
+      <c r="B41" s="5" t="inlineStr">
         <is>
           <t>Kowalska</t>
         </is>
       </c>
-      <c r="C41" s="2" t="inlineStr">
+      <c r="C41" s="3" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
+      <c r="D41" s="2" t="n"/>
+      <c r="E41" s="2" t="n"/>
+      <c r="F41" s="5" t="n"/>
+      <c r="G41" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" ht="18.75" customHeight="1">
-      <c r="A42" s="2" t="inlineStr">
+      <c r="A42" s="5" t="inlineStr">
         <is>
           <t>Marcin</t>
         </is>
       </c>
-      <c r="B42" s="2" t="inlineStr">
+      <c r="B42" s="5" t="inlineStr">
         <is>
           <t>Lis</t>
         </is>
       </c>
-      <c r="C42" s="2" t="inlineStr">
+      <c r="C42" s="3" t="inlineStr">
         <is>
           <t>M. L.</t>
         </is>
       </c>
+      <c r="D42" s="2" t="n"/>
+      <c r="E42" s="2" t="n"/>
+      <c r="F42" s="5" t="n"/>
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" ht="18.75" customHeight="1">
-      <c r="A43" s="2" t="inlineStr">
+      <c r="A43" s="5" t="inlineStr">
         <is>
           <t>Jadwiga</t>
         </is>
       </c>
-      <c r="B43" s="2" t="inlineStr">
+      <c r="B43" s="5" t="inlineStr">
         <is>
           <t>Ziółkowska</t>
         </is>
       </c>
-      <c r="C43" s="2" t="inlineStr">
+      <c r="C43" s="3" t="inlineStr">
         <is>
           <t>J. Z.</t>
         </is>
       </c>
+      <c r="D43" s="2" t="n"/>
+      <c r="E43" s="2" t="n"/>
+      <c r="F43" s="5" t="n"/>
+      <c r="G43" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" ht="18.75" customHeight="1">
-      <c r="A44" s="2" t="inlineStr">
+      <c r="A44" s="5" t="inlineStr">
         <is>
           <t>Sławomir</t>
         </is>
       </c>
-      <c r="B44" s="2" t="inlineStr">
+      <c r="B44" s="5" t="inlineStr">
         <is>
           <t>Jankowski</t>
         </is>
       </c>
-      <c r="C44" s="2" t="inlineStr">
+      <c r="C44" s="3" t="inlineStr">
         <is>
           <t>S. J.</t>
         </is>
       </c>
+      <c r="D44" s="2" t="n"/>
+      <c r="E44" s="2" t="n"/>
+      <c r="F44" s="5" t="n"/>
+      <c r="G44" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" ht="18.75" customHeight="1">
-      <c r="A45" s="2" t="inlineStr">
+      <c r="A45" s="5" t="inlineStr">
         <is>
           <t>Teresa</t>
         </is>
       </c>
-      <c r="B45" s="2" t="inlineStr">
+      <c r="B45" s="5" t="inlineStr">
         <is>
           <t>Piotrowska</t>
         </is>
       </c>
-      <c r="C45" s="2" t="inlineStr">
+      <c r="C45" s="3" t="inlineStr">
         <is>
           <t>T. P.</t>
         </is>
       </c>
+      <c r="D45" s="2" t="n"/>
+      <c r="E45" s="2" t="n"/>
+      <c r="F45" s="5" t="n"/>
+      <c r="G45" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" ht="18.75" customHeight="1">
-      <c r="A46" s="2" t="inlineStr">
+      <c r="A46" s="5" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B46" s="2" t="inlineStr">
+      <c r="B46" s="5" t="inlineStr">
         <is>
           <t>Przybylski</t>
         </is>
       </c>
-      <c r="C46" s="2" t="inlineStr">
+      <c r="C46" s="3" t="inlineStr">
         <is>
           <t>P. P.</t>
         </is>
       </c>
+      <c r="D46" s="2" t="n"/>
+      <c r="E46" s="2" t="n"/>
+      <c r="F46" s="5" t="n"/>
+      <c r="G46" s="2" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="47" ht="18.75" customHeight="1">
-      <c r="A47" s="2" t="inlineStr">
+      <c r="A47" s="5" t="inlineStr">
         <is>
           <t>Ryszard</t>
         </is>
       </c>
-      <c r="B47" s="2" t="inlineStr">
+      <c r="B47" s="5" t="inlineStr">
         <is>
           <t>Nowicki</t>
         </is>
       </c>
-      <c r="C47" s="2" t="inlineStr">
+      <c r="C47" s="3" t="inlineStr">
         <is>
           <t>R. N.</t>
         </is>
       </c>
+      <c r="D47" s="2" t="n"/>
+      <c r="E47" s="2" t="n"/>
+      <c r="F47" s="5" t="n"/>
+      <c r="G47" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" ht="18.75" customHeight="1">
-      <c r="A48" s="2" t="inlineStr">
+      <c r="A48" s="5" t="inlineStr">
         <is>
           <t>Marcin</t>
         </is>
       </c>
-      <c r="B48" s="2" t="inlineStr">
+      <c r="B48" s="5" t="inlineStr">
         <is>
           <t>Borkowski</t>
         </is>
       </c>
-      <c r="C48" s="2" t="inlineStr">
+      <c r="C48" s="3" t="inlineStr">
         <is>
           <t>M. B.</t>
         </is>
       </c>
+      <c r="D48" s="2" t="n"/>
+      <c r="E48" s="2" t="n"/>
+      <c r="F48" s="5" t="n"/>
+      <c r="G48" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" ht="18.75" customHeight="1">
-      <c r="A49" s="2" t="inlineStr">
+      <c r="A49" s="5" t="inlineStr">
         <is>
           <t>Sylwia</t>
         </is>
       </c>
-      <c r="B49" s="2" t="inlineStr">
+      <c r="B49" s="5" t="inlineStr">
         <is>
           <t>Gajewska</t>
         </is>
       </c>
-      <c r="C49" s="2" t="inlineStr">
+      <c r="C49" s="3" t="inlineStr">
         <is>
           <t>S. G.</t>
         </is>
       </c>
+      <c r="D49" s="2" t="n"/>
+      <c r="E49" s="2" t="n"/>
+      <c r="F49" s="5" t="n"/>
+      <c r="G49" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" ht="18.75" customHeight="1">
-      <c r="A50" s="2" t="inlineStr">
+      <c r="A50" s="5" t="inlineStr">
         <is>
           <t>Tadeusz</t>
         </is>
       </c>
-      <c r="B50" s="2" t="inlineStr">
+      <c r="B50" s="5" t="inlineStr">
         <is>
           <t>Malinowski</t>
         </is>
       </c>
-      <c r="C50" s="2" t="inlineStr">
+      <c r="C50" s="3" t="inlineStr">
         <is>
           <t>T. M.</t>
         </is>
       </c>
+      <c r="D50" s="2" t="n"/>
+      <c r="E50" s="2" t="n"/>
+      <c r="F50" s="5" t="n"/>
+      <c r="G50" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" ht="18.75" customHeight="1">
-      <c r="A51" s="2" t="inlineStr">
+      <c r="A51" s="5" t="inlineStr">
         <is>
           <t>Marta</t>
         </is>
       </c>
-      <c r="B51" s="2" t="inlineStr">
+      <c r="B51" s="5" t="inlineStr">
         <is>
           <t>Wieczorek</t>
         </is>
       </c>
-      <c r="C51" s="2" t="inlineStr">
+      <c r="C51" s="3" t="inlineStr">
         <is>
           <t>M. W.</t>
         </is>
       </c>
+      <c r="D51" s="2" t="n"/>
+      <c r="E51" s="2" t="n"/>
+      <c r="F51" s="5" t="n"/>
+      <c r="G51" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" ht="18.75" customHeight="1">
-      <c r="A52" s="2" t="inlineStr">
+      <c r="A52" s="5" t="inlineStr">
         <is>
           <t>Kamil</t>
         </is>
       </c>
-      <c r="B52" s="2" t="inlineStr">
+      <c r="B52" s="5" t="inlineStr">
         <is>
           <t>Pawłowski</t>
         </is>
       </c>
-      <c r="C52" s="2" t="inlineStr">
+      <c r="C52" s="3" t="inlineStr">
         <is>
           <t>K. P.</t>
         </is>
       </c>
+      <c r="D52" s="2" t="n"/>
+      <c r="E52" s="2" t="n"/>
+      <c r="F52" s="5" t="n"/>
+      <c r="G52" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" ht="18.75" customHeight="1">
-      <c r="A53" s="2" t="inlineStr">
+      <c r="A53" s="5" t="inlineStr">
         <is>
           <t>Halina</t>
         </is>
       </c>
-      <c r="B53" s="2" t="inlineStr">
+      <c r="B53" s="5" t="inlineStr">
         <is>
           <t>Urbańska</t>
         </is>
       </c>
-      <c r="C53" s="2" t="inlineStr">
+      <c r="C53" s="3" t="inlineStr">
         <is>
           <t>H. U.</t>
         </is>
       </c>
+      <c r="D53" s="2" t="n"/>
+      <c r="E53" s="2" t="n"/>
+      <c r="F53" s="5" t="n"/>
+      <c r="G53" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" ht="18.75" customHeight="1">
-      <c r="A54" s="2" t="inlineStr">
+      <c r="A54" s="5" t="inlineStr">
         <is>
           <t>Beata</t>
         </is>
       </c>
-      <c r="B54" s="2" t="inlineStr">
+      <c r="B54" s="5" t="inlineStr">
         <is>
           <t>Pietrzak</t>
         </is>
       </c>
-      <c r="C54" s="2" t="inlineStr">
+      <c r="C54" s="3" t="inlineStr">
         <is>
           <t>B. P.</t>
         </is>
       </c>
+      <c r="D54" s="2" t="n"/>
+      <c r="E54" s="2" t="n"/>
+      <c r="F54" s="5" t="n"/>
+      <c r="G54" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" ht="18.75" customHeight="1">
-      <c r="A55" s="2" t="inlineStr">
+      <c r="A55" s="5" t="inlineStr">
         <is>
           <t>Marianna</t>
         </is>
       </c>
-      <c r="B55" s="2" t="inlineStr">
+      <c r="B55" s="5" t="inlineStr">
         <is>
           <t>Wójcik</t>
         </is>
       </c>
-      <c r="C55" s="2" t="inlineStr">
+      <c r="C55" s="3" t="inlineStr">
         <is>
           <t>M. W.</t>
         </is>
       </c>
+      <c r="D55" s="2" t="n"/>
+      <c r="E55" s="2" t="n"/>
+      <c r="F55" s="5" t="n"/>
+      <c r="G55" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" ht="18.75" customHeight="1">
-      <c r="A56" s="2" t="inlineStr">
+      <c r="A56" s="5" t="inlineStr">
         <is>
           <t>Ewelina</t>
         </is>
       </c>
-      <c r="B56" s="2" t="inlineStr">
+      <c r="B56" s="5" t="inlineStr">
         <is>
           <t>Górska</t>
         </is>
       </c>
-      <c r="C56" s="2" t="inlineStr">
+      <c r="C56" s="3" t="inlineStr">
         <is>
           <t>E. G.</t>
         </is>
       </c>
+      <c r="D56" s="2" t="n"/>
+      <c r="E56" s="2" t="n"/>
+      <c r="F56" s="5" t="n"/>
+      <c r="G56" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" ht="18.75" customHeight="1">
-      <c r="A57" s="2" t="inlineStr">
+      <c r="A57" s="5" t="inlineStr">
         <is>
           <t>Krzysztof</t>
         </is>
       </c>
-      <c r="B57" s="2" t="inlineStr">
+      <c r="B57" s="5" t="inlineStr">
         <is>
           <t>Michalak</t>
         </is>
       </c>
-      <c r="C57" s="2" t="inlineStr">
+      <c r="C57" s="3" t="inlineStr">
         <is>
           <t>K. M.</t>
         </is>
       </c>
+      <c r="D57" s="2" t="n"/>
+      <c r="E57" s="2" t="n"/>
+      <c r="F57" s="5" t="n"/>
+      <c r="G57" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" ht="18.75" customHeight="1">
-      <c r="A58" s="2" t="inlineStr">
+      <c r="A58" s="5" t="inlineStr">
         <is>
           <t>Ewa</t>
         </is>
       </c>
-      <c r="B58" s="2" t="inlineStr">
+      <c r="B58" s="5" t="inlineStr">
         <is>
           <t>Dąbrowska</t>
         </is>
       </c>
-      <c r="C58" s="2" t="inlineStr">
+      <c r="C58" s="3" t="inlineStr">
         <is>
           <t>E. D.</t>
         </is>
       </c>
+      <c r="D58" s="2" t="n"/>
+      <c r="E58" s="2" t="n"/>
+      <c r="F58" s="5" t="n"/>
+      <c r="G58" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" ht="18.75" customHeight="1">
-      <c r="A59" s="2" t="inlineStr">
+      <c r="A59" s="5" t="inlineStr">
         <is>
           <t>Andrzej</t>
         </is>
       </c>
-      <c r="B59" s="2" t="inlineStr">
+      <c r="B59" s="5" t="inlineStr">
         <is>
           <t>Wieczorek</t>
         </is>
       </c>
-      <c r="C59" s="2" t="inlineStr">
+      <c r="C59" s="3" t="inlineStr">
         <is>
           <t>A. W.</t>
         </is>
       </c>
+      <c r="D59" s="2" t="n"/>
+      <c r="E59" s="2" t="n"/>
+      <c r="F59" s="5" t="n"/>
+      <c r="G59" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" ht="18.75" customHeight="1">
-      <c r="A60" s="2" t="inlineStr">
+      <c r="A60" s="5" t="inlineStr">
         <is>
           <t>Elżbieta</t>
         </is>
       </c>
-      <c r="B60" s="2" t="inlineStr">
+      <c r="B60" s="5" t="inlineStr">
         <is>
           <t>Wiśniewska</t>
         </is>
       </c>
-      <c r="C60" s="2" t="inlineStr">
+      <c r="C60" s="3" t="inlineStr">
         <is>
           <t>E. W.</t>
         </is>
       </c>
+      <c r="D60" s="2" t="n"/>
+      <c r="E60" s="2" t="n"/>
+      <c r="F60" s="5" t="n"/>
+      <c r="G60" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" ht="18.75" customHeight="1">
-      <c r="A61" s="2" t="inlineStr">
+      <c r="A61" s="5" t="inlineStr">
         <is>
           <t>Grażyna</t>
         </is>
       </c>
-      <c r="B61" s="2" t="inlineStr">
+      <c r="B61" s="5" t="inlineStr">
         <is>
           <t>Zakrzewska</t>
         </is>
       </c>
-      <c r="C61" s="2" t="inlineStr">
+      <c r="C61" s="3" t="inlineStr">
         <is>
           <t>G. Z.</t>
         </is>
       </c>
+      <c r="D61" s="2" t="n"/>
+      <c r="E61" s="2" t="n"/>
+      <c r="F61" s="5" t="n"/>
+      <c r="G61" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" ht="18.75" customHeight="1">
-      <c r="A62" s="2" t="inlineStr">
+      <c r="A62" s="5" t="inlineStr">
         <is>
           <t>Monika</t>
         </is>
       </c>
-      <c r="B62" s="2" t="inlineStr">
+      <c r="B62" s="5" t="inlineStr">
         <is>
           <t>Kamińska</t>
         </is>
       </c>
-      <c r="C62" s="2" t="inlineStr">
+      <c r="C62" s="3" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
+      <c r="D62" s="2" t="n"/>
+      <c r="E62" s="2" t="n"/>
+      <c r="F62" s="5" t="n"/>
+      <c r="G62" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" ht="18.75" customHeight="1">
-      <c r="A63" s="2" t="inlineStr">
+      <c r="A63" s="5" t="inlineStr">
         <is>
           <t>Alicja</t>
         </is>
       </c>
-      <c r="B63" s="2" t="inlineStr">
+      <c r="B63" s="5" t="inlineStr">
         <is>
           <t>Kozłowska</t>
         </is>
       </c>
-      <c r="C63" s="2" t="inlineStr">
+      <c r="C63" s="3" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
+      <c r="D63" s="2" t="n"/>
+      <c r="E63" s="2" t="n"/>
+      <c r="F63" s="5" t="n"/>
+      <c r="G63" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" ht="18.75" customHeight="1">
-      <c r="A64" s="2" t="inlineStr">
+      <c r="A64" s="5" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B64" s="2" t="inlineStr">
+      <c r="B64" s="5" t="inlineStr">
         <is>
           <t>Nowakowski</t>
         </is>
       </c>
-      <c r="C64" s="2" t="inlineStr">
+      <c r="C64" s="3" t="inlineStr">
         <is>
           <t>P. N.</t>
         </is>
       </c>
+      <c r="D64" s="2" t="n"/>
+      <c r="E64" s="2" t="n"/>
+      <c r="F64" s="5" t="n"/>
+      <c r="G64" s="2" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="65" ht="18.75" customHeight="1">
-      <c r="A65" s="2" t="inlineStr">
+      <c r="A65" s="5" t="inlineStr">
         <is>
           <t>Katarzyna</t>
         </is>
       </c>
-      <c r="B65" s="2" t="inlineStr">
+      <c r="B65" s="5" t="inlineStr">
         <is>
           <t>Gajewska</t>
         </is>
       </c>
-      <c r="C65" s="2" t="inlineStr">
+      <c r="C65" s="3" t="inlineStr">
         <is>
           <t>K. G.</t>
         </is>
       </c>
+      <c r="D65" s="2" t="n"/>
+      <c r="E65" s="2" t="n"/>
+      <c r="F65" s="5" t="n"/>
+      <c r="G65" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" ht="18.75" customHeight="1">
-      <c r="A66" s="2" t="inlineStr">
+      <c r="A66" s="5" t="inlineStr">
         <is>
           <t>Agata</t>
         </is>
       </c>
-      <c r="B66" s="2" t="inlineStr">
+      <c r="B66" s="5" t="inlineStr">
         <is>
           <t>Pietrzak</t>
         </is>
       </c>
-      <c r="C66" s="2" t="inlineStr">
+      <c r="C66" s="3" t="inlineStr">
         <is>
           <t>A. P.</t>
         </is>
       </c>
+      <c r="D66" s="2" t="n"/>
+      <c r="E66" s="2" t="n"/>
+      <c r="F66" s="5" t="n"/>
+      <c r="G66" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" ht="18.75" customHeight="1">
-      <c r="A67" s="2" t="inlineStr">
+      <c r="A67" s="5" t="inlineStr">
         <is>
           <t>Edward</t>
         </is>
       </c>
-      <c r="B67" s="2" t="inlineStr">
+      <c r="B67" s="5" t="inlineStr">
         <is>
           <t>Jankowski</t>
         </is>
       </c>
-      <c r="C67" s="2" t="inlineStr">
+      <c r="C67" s="3" t="inlineStr">
         <is>
           <t>E. J.</t>
         </is>
       </c>
+      <c r="D67" s="2" t="n"/>
+      <c r="E67" s="2" t="n"/>
+      <c r="F67" s="5" t="n"/>
+      <c r="G67" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" ht="18.75" customHeight="1">
-      <c r="A68" s="2" t="inlineStr">
+      <c r="A68" s="5" t="inlineStr">
         <is>
           <t>Jakub</t>
         </is>
       </c>
-      <c r="B68" s="2" t="inlineStr">
+      <c r="B68" s="5" t="inlineStr">
         <is>
           <t>Krajewski</t>
         </is>
       </c>
-      <c r="C68" s="2" t="inlineStr">
+      <c r="C68" s="3" t="inlineStr">
         <is>
           <t>J. K.</t>
         </is>
       </c>
+      <c r="D68" s="2" t="n"/>
+      <c r="E68" s="2" t="n"/>
+      <c r="F68" s="5" t="n"/>
+      <c r="G68" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" ht="18.75" customHeight="1">
-      <c r="A69" s="2" t="inlineStr">
+      <c r="A69" s="5" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="B69" s="2" t="inlineStr">
+      <c r="B69" s="5" t="inlineStr">
         <is>
           <t>Szulc</t>
         </is>
       </c>
-      <c r="C69" s="2" t="inlineStr">
+      <c r="C69" s="3" t="inlineStr">
         <is>
           <t>J. S.</t>
         </is>
       </c>
+      <c r="D69" s="2" t="n"/>
+      <c r="E69" s="2" t="n"/>
+      <c r="F69" s="5" t="n"/>
+      <c r="G69" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" ht="18.75" customHeight="1">
-      <c r="A70" s="2" t="inlineStr">
+      <c r="A70" s="5" t="inlineStr">
         <is>
           <t>Alicja</t>
         </is>
       </c>
-      <c r="B70" s="2" t="inlineStr">
+      <c r="B70" s="5" t="inlineStr">
         <is>
           <t>Krajewska</t>
         </is>
       </c>
-      <c r="C70" s="2" t="inlineStr">
+      <c r="C70" s="3" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
+      <c r="D70" s="2" t="n"/>
+      <c r="E70" s="2" t="n"/>
+      <c r="F70" s="5" t="n"/>
+      <c r="G70" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" ht="18.75" customHeight="1">
-      <c r="A71" s="2" t="inlineStr">
+      <c r="A71" s="5" t="inlineStr">
         <is>
           <t>Stefania</t>
         </is>
       </c>
-      <c r="B71" s="2" t="inlineStr">
+      <c r="B71" s="5" t="inlineStr">
         <is>
           <t>Adamczyk</t>
         </is>
       </c>
-      <c r="C71" s="2" t="inlineStr">
+      <c r="C71" s="3" t="inlineStr">
         <is>
           <t>S. A.</t>
         </is>
       </c>
+      <c r="D71" s="2" t="n"/>
+      <c r="E71" s="2" t="n"/>
+      <c r="F71" s="5" t="n"/>
+      <c r="G71" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" ht="18.75" customHeight="1">
-      <c r="A72" s="2" t="inlineStr">
+      <c r="A72" s="5" t="inlineStr">
         <is>
           <t>Daniel</t>
         </is>
       </c>
-      <c r="B72" s="2" t="inlineStr">
+      <c r="B72" s="5" t="inlineStr">
         <is>
           <t>Majewski</t>
         </is>
       </c>
-      <c r="C72" s="2" t="inlineStr">
+      <c r="C72" s="3" t="inlineStr">
         <is>
           <t>D. M.</t>
         </is>
       </c>
+      <c r="D72" s="2" t="n"/>
+      <c r="E72" s="2" t="n"/>
+      <c r="F72" s="5" t="n"/>
+      <c r="G72" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" ht="18.75" customHeight="1">
-      <c r="A73" s="2" t="inlineStr">
+      <c r="A73" s="5" t="inlineStr">
         <is>
           <t>Leszek</t>
         </is>
       </c>
-      <c r="B73" s="2" t="inlineStr">
+      <c r="B73" s="5" t="inlineStr">
         <is>
           <t>Wasilewski</t>
         </is>
       </c>
-      <c r="C73" s="2" t="inlineStr">
+      <c r="C73" s="3" t="inlineStr">
         <is>
           <t>L. W.</t>
         </is>
       </c>
+      <c r="D73" s="2" t="n"/>
+      <c r="E73" s="2" t="n"/>
+      <c r="F73" s="5" t="n"/>
+      <c r="G73" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" ht="18.75" customHeight="1">
-      <c r="A74" s="2" t="inlineStr">
+      <c r="A74" s="5" t="inlineStr">
         <is>
           <t>Maria</t>
         </is>
       </c>
-      <c r="B74" s="2" t="inlineStr">
+      <c r="B74" s="5" t="inlineStr">
         <is>
           <t>Kucharska</t>
         </is>
       </c>
-      <c r="C74" s="2" t="inlineStr">
+      <c r="C74" s="3" t="inlineStr">
         <is>
           <t>M. K.</t>
         </is>
       </c>
+      <c r="D74" s="2" t="n"/>
+      <c r="E74" s="2" t="n"/>
+      <c r="F74" s="5" t="n"/>
+      <c r="G74" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" ht="18.75" customHeight="1">
-      <c r="A75" s="2" t="inlineStr">
+      <c r="A75" s="5" t="inlineStr">
         <is>
           <t>Dawid</t>
         </is>
       </c>
-      <c r="B75" s="2" t="inlineStr">
+      <c r="B75" s="5" t="inlineStr">
         <is>
           <t>Szulc</t>
         </is>
       </c>
-      <c r="C75" s="2" t="inlineStr">
+      <c r="C75" s="3" t="inlineStr">
         <is>
           <t>D. S.</t>
         </is>
       </c>
+      <c r="D75" s="2" t="n"/>
+      <c r="E75" s="2" t="n"/>
+      <c r="F75" s="5" t="n"/>
+      <c r="G75" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" ht="18.75" customHeight="1">
-      <c r="A76" s="2" t="inlineStr">
+      <c r="A76" s="5" t="inlineStr">
         <is>
           <t>Sławomir</t>
         </is>
       </c>
-      <c r="B76" s="2" t="inlineStr">
+      <c r="B76" s="5" t="inlineStr">
         <is>
           <t>Zając</t>
         </is>
       </c>
-      <c r="C76" s="2" t="inlineStr">
+      <c r="C76" s="3" t="inlineStr">
         <is>
           <t>S. Z.</t>
         </is>
       </c>
+      <c r="D76" s="2" t="n"/>
+      <c r="E76" s="2" t="n"/>
+      <c r="F76" s="5" t="n"/>
+      <c r="G76" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" ht="18.75" customHeight="1">
-      <c r="A77" s="2" t="inlineStr">
+      <c r="A77" s="5" t="inlineStr">
         <is>
           <t>Monika</t>
         </is>
       </c>
-      <c r="B77" s="2" t="inlineStr">
+      <c r="B77" s="5" t="inlineStr">
         <is>
           <t>Nowakowska</t>
         </is>
       </c>
-      <c r="C77" s="2" t="inlineStr">
+      <c r="C77" s="3" t="inlineStr">
         <is>
           <t>M. N.</t>
         </is>
       </c>
+      <c r="D77" s="2" t="n"/>
+      <c r="E77" s="2" t="n"/>
+      <c r="F77" s="5" t="n"/>
+      <c r="G77" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" ht="18.75" customHeight="1">
-      <c r="A78" s="2" t="inlineStr">
+      <c r="A78" s="5" t="inlineStr">
         <is>
           <t>Leszek</t>
         </is>
       </c>
-      <c r="B78" s="2" t="inlineStr">
+      <c r="B78" s="5" t="inlineStr">
         <is>
           <t>Brzeziński</t>
         </is>
       </c>
-      <c r="C78" s="2" t="inlineStr">
+      <c r="C78" s="3" t="inlineStr">
         <is>
           <t>L. B.</t>
         </is>
       </c>
+      <c r="D78" s="2" t="n"/>
+      <c r="E78" s="2" t="n"/>
+      <c r="F78" s="5" t="n"/>
+      <c r="G78" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" ht="18.75" customHeight="1">
-      <c r="A79" s="2" t="inlineStr">
+      <c r="A79" s="5" t="inlineStr">
         <is>
           <t>Jarosław</t>
         </is>
       </c>
-      <c r="B79" s="2" t="inlineStr">
+      <c r="B79" s="5" t="inlineStr">
         <is>
           <t>Majewski</t>
         </is>
       </c>
-      <c r="C79" s="2" t="inlineStr">
+      <c r="C79" s="3" t="inlineStr">
         <is>
           <t>J. M.</t>
         </is>
       </c>
+      <c r="D79" s="2" t="n"/>
+      <c r="E79" s="2" t="n"/>
+      <c r="F79" s="5" t="n"/>
+      <c r="G79" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" ht="18.75" customHeight="1">
-      <c r="A80" s="2" t="inlineStr">
+      <c r="A80" s="5" t="inlineStr">
         <is>
           <t>Mariusz</t>
         </is>
       </c>
-      <c r="B80" s="2" t="inlineStr">
+      <c r="B80" s="5" t="inlineStr">
         <is>
           <t>Majewski</t>
         </is>
       </c>
-      <c r="C80" s="2" t="inlineStr">
+      <c r="C80" s="3" t="inlineStr">
         <is>
           <t>M. M.</t>
         </is>
       </c>
+      <c r="D80" s="2" t="n"/>
+      <c r="E80" s="2" t="n"/>
+      <c r="F80" s="5" t="n"/>
+      <c r="G80" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" ht="18.75" customHeight="1">
-      <c r="A81" s="2" t="inlineStr">
+      <c r="A81" s="5" t="inlineStr">
         <is>
           <t>Stanisław</t>
         </is>
       </c>
-      <c r="B81" s="2" t="inlineStr">
+      <c r="B81" s="5" t="inlineStr">
         <is>
           <t>Baran</t>
         </is>
       </c>
-      <c r="C81" s="2" t="inlineStr">
+      <c r="C81" s="3" t="inlineStr">
         <is>
           <t>S. B.</t>
         </is>
       </c>
+      <c r="D81" s="2" t="n"/>
+      <c r="E81" s="2" t="n"/>
+      <c r="F81" s="5" t="n"/>
+      <c r="G81" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" ht="18.75" customHeight="1">
-      <c r="A82" s="2" t="inlineStr">
+      <c r="A82" s="5" t="inlineStr">
         <is>
           <t>Andrzej</t>
         </is>
       </c>
-      <c r="B82" s="2" t="inlineStr">
+      <c r="B82" s="5" t="inlineStr">
         <is>
           <t>Dąbrowski</t>
         </is>
       </c>
-      <c r="C82" s="2" t="inlineStr">
+      <c r="C82" s="3" t="inlineStr">
         <is>
           <t>A. D.</t>
         </is>
       </c>
+      <c r="D82" s="2" t="n"/>
+      <c r="E82" s="2" t="n"/>
+      <c r="F82" s="5" t="n"/>
+      <c r="G82" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" ht="18.75" customHeight="1">
-      <c r="A83" s="2" t="inlineStr">
+      <c r="A83" s="5" t="inlineStr">
         <is>
           <t>Dawid</t>
         </is>
       </c>
-      <c r="B83" s="2" t="inlineStr">
+      <c r="B83" s="5" t="inlineStr">
         <is>
           <t>Sobczak</t>
         </is>
       </c>
-      <c r="C83" s="2" t="inlineStr">
+      <c r="C83" s="3" t="inlineStr">
         <is>
           <t>D. S.</t>
         </is>
       </c>
+      <c r="D83" s="2" t="n"/>
+      <c r="E83" s="2" t="n"/>
+      <c r="F83" s="5" t="n"/>
+      <c r="G83" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" ht="18.75" customHeight="1">
-      <c r="A84" s="2" t="inlineStr">
+      <c r="A84" s="5" t="inlineStr">
         <is>
           <t>Magdalena</t>
         </is>
       </c>
-      <c r="B84" s="2" t="inlineStr">
+      <c r="B84" s="5" t="inlineStr">
         <is>
           <t>Lis</t>
         </is>
       </c>
-      <c r="C84" s="2" t="inlineStr">
+      <c r="C84" s="3" t="inlineStr">
         <is>
           <t>M. L.</t>
         </is>
       </c>
+      <c r="D84" s="2" t="n"/>
+      <c r="E84" s="2" t="n"/>
+      <c r="F84" s="5" t="n"/>
+      <c r="G84" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" ht="18.75" customHeight="1">
-      <c r="A85" s="2" t="inlineStr">
+      <c r="A85" s="5" t="inlineStr">
         <is>
           <t>Karolina</t>
         </is>
       </c>
-      <c r="B85" s="2" t="inlineStr">
+      <c r="B85" s="5" t="inlineStr">
         <is>
           <t>Zając</t>
         </is>
       </c>
-      <c r="C85" s="2" t="inlineStr">
+      <c r="C85" s="3" t="inlineStr">
         <is>
           <t>K. Z.</t>
         </is>
       </c>
+      <c r="D85" s="2" t="n"/>
+      <c r="E85" s="2" t="n"/>
+      <c r="F85" s="5" t="n"/>
+      <c r="G85" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" ht="18.75" customHeight="1">
-      <c r="A86" s="2" t="inlineStr">
+      <c r="A86" s="5" t="inlineStr">
         <is>
           <t>Adam</t>
         </is>
       </c>
-      <c r="B86" s="2" t="inlineStr">
+      <c r="B86" s="5" t="inlineStr">
         <is>
           <t>Kaczmarek</t>
         </is>
       </c>
-      <c r="C86" s="2" t="inlineStr">
+      <c r="C86" s="3" t="inlineStr">
         <is>
           <t>A. K.</t>
         </is>
       </c>
+      <c r="D86" s="2" t="n"/>
+      <c r="E86" s="2" t="n"/>
+      <c r="F86" s="5" t="n"/>
+      <c r="G86" s="2" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="87" ht="18.75" customHeight="1">
-      <c r="A87" s="2" t="inlineStr">
+      <c r="A87" s="5" t="inlineStr">
         <is>
           <t>Czesław</t>
         </is>
       </c>
-      <c r="B87" s="2" t="inlineStr">
+      <c r="B87" s="5" t="inlineStr">
         <is>
           <t>Kowalczyk</t>
         </is>
       </c>
-      <c r="C87" s="2" t="inlineStr">
+      <c r="C87" s="3" t="inlineStr">
         <is>
           <t>C. K.</t>
         </is>
       </c>
+      <c r="D87" s="2" t="n"/>
+      <c r="E87" s="2" t="n"/>
+      <c r="F87" s="5" t="n"/>
+      <c r="G87" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" ht="18.75" customHeight="1">
-      <c r="A88" s="2" t="inlineStr">
+      <c r="A88" s="5" t="inlineStr">
         <is>
           <t>Łukasz</t>
         </is>
       </c>
-      <c r="B88" s="2" t="inlineStr">
+      <c r="B88" s="5" t="inlineStr">
         <is>
           <t>Jaworski</t>
         </is>
       </c>
-      <c r="C88" s="2" t="inlineStr">
+      <c r="C88" s="3" t="inlineStr">
         <is>
           <t>Ł. J.</t>
         </is>
       </c>
+      <c r="D88" s="2" t="n"/>
+      <c r="E88" s="2" t="n"/>
+      <c r="F88" s="5" t="n"/>
+      <c r="G88" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" ht="18.75" customHeight="1">
-      <c r="A89" s="2" t="inlineStr">
+      <c r="A89" s="5" t="inlineStr">
         <is>
           <t>Marta</t>
         </is>
       </c>
-      <c r="B89" s="2" t="inlineStr">
+      <c r="B89" s="5" t="inlineStr">
         <is>
           <t>Jakubowska</t>
         </is>
       </c>
-      <c r="C89" s="2" t="inlineStr">
+      <c r="C89" s="3" t="inlineStr">
         <is>
           <t>M. J.</t>
         </is>
       </c>
+      <c r="D89" s="2" t="n"/>
+      <c r="E89" s="2" t="n"/>
+      <c r="F89" s="5" t="n"/>
+      <c r="G89" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" ht="18.75" customHeight="1">
-      <c r="A90" s="2" t="inlineStr">
+      <c r="A90" s="5" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B90" s="2" t="inlineStr">
+      <c r="B90" s="5" t="inlineStr">
         <is>
           <t>Woźniak</t>
         </is>
       </c>
-      <c r="C90" s="2" t="inlineStr">
+      <c r="C90" s="3" t="inlineStr">
         <is>
           <t>P. W.</t>
         </is>
       </c>
+      <c r="D90" s="2" t="n"/>
+      <c r="E90" s="2" t="n"/>
+      <c r="F90" s="5" t="n"/>
+      <c r="G90" s="2" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="91" ht="18.75" customHeight="1">
-      <c r="A91" s="2" t="inlineStr">
+      <c r="A91" s="5" t="inlineStr">
         <is>
           <t>Monika</t>
         </is>
       </c>
-      <c r="B91" s="2" t="inlineStr">
+      <c r="B91" s="5" t="inlineStr">
         <is>
           <t>Zając</t>
         </is>
       </c>
-      <c r="C91" s="2" t="inlineStr">
+      <c r="C91" s="3" t="inlineStr">
         <is>
           <t>M. Z.</t>
         </is>
       </c>
+      <c r="D91" s="2" t="n"/>
+      <c r="E91" s="2" t="n"/>
+      <c r="F91" s="5" t="n"/>
+      <c r="G91" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" ht="18.75" customHeight="1">
-      <c r="A92" s="2" t="inlineStr">
+      <c r="A92" s="5" t="inlineStr">
         <is>
           <t>Waldemar</t>
         </is>
       </c>
-      <c r="B92" s="2" t="inlineStr">
+      <c r="B92" s="5" t="inlineStr">
         <is>
           <t>Witkowski</t>
         </is>
       </c>
-      <c r="C92" s="2" t="inlineStr">
+      <c r="C92" s="3" t="inlineStr">
         <is>
           <t>W. W.</t>
         </is>
       </c>
+      <c r="D92" s="2" t="n"/>
+      <c r="E92" s="2" t="n"/>
+      <c r="F92" s="5" t="n"/>
+      <c r="G92" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" ht="18.75" customHeight="1">
-      <c r="A93" s="2" t="inlineStr">
+      <c r="A93" s="5" t="inlineStr">
         <is>
           <t>Izabela</t>
         </is>
       </c>
-      <c r="B93" s="2" t="inlineStr">
+      <c r="B93" s="5" t="inlineStr">
         <is>
           <t>Król</t>
         </is>
       </c>
-      <c r="C93" s="2" t="inlineStr">
+      <c r="C93" s="3" t="inlineStr">
         <is>
           <t>I. K.</t>
         </is>
       </c>
+      <c r="D93" s="2" t="n"/>
+      <c r="E93" s="2" t="n"/>
+      <c r="F93" s="5" t="n"/>
+      <c r="G93" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" ht="18.75" customHeight="1">
-      <c r="A94" s="2" t="inlineStr">
+      <c r="A94" s="5" t="inlineStr">
         <is>
           <t>Mateusz</t>
         </is>
       </c>
-      <c r="B94" s="2" t="inlineStr">
+      <c r="B94" s="5" t="inlineStr">
         <is>
           <t>Przybylski</t>
         </is>
       </c>
-      <c r="C94" s="2" t="inlineStr">
+      <c r="C94" s="3" t="inlineStr">
         <is>
           <t>M. P.</t>
         </is>
       </c>
+      <c r="D94" s="2" t="n"/>
+      <c r="E94" s="2" t="n"/>
+      <c r="F94" s="5" t="n"/>
+      <c r="G94" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" ht="18.75" customHeight="1">
-      <c r="A95" s="2" t="inlineStr">
+      <c r="A95" s="5" t="inlineStr">
         <is>
           <t>Stanisław</t>
         </is>
       </c>
-      <c r="B95" s="2" t="inlineStr">
+      <c r="B95" s="5" t="inlineStr">
         <is>
           <t>Jasiński</t>
         </is>
       </c>
-      <c r="C95" s="2" t="inlineStr">
+      <c r="C95" s="3" t="inlineStr">
         <is>
           <t>S. J.</t>
         </is>
       </c>
+      <c r="D95" s="2" t="n"/>
+      <c r="E95" s="2" t="n"/>
+      <c r="F95" s="5" t="n"/>
+      <c r="G95" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" ht="18.75" customHeight="1">
-      <c r="A96" s="2" t="inlineStr">
+      <c r="A96" s="5" t="inlineStr">
         <is>
           <t>Wiesława</t>
         </is>
       </c>
-      <c r="B96" s="2" t="inlineStr">
+      <c r="B96" s="5" t="inlineStr">
         <is>
           <t>Adamska</t>
         </is>
       </c>
-      <c r="C96" s="2" t="inlineStr">
+      <c r="C96" s="3" t="inlineStr">
         <is>
           <t>W. A.</t>
         </is>
       </c>
+      <c r="D96" s="2" t="n"/>
+      <c r="E96" s="2" t="n"/>
+      <c r="F96" s="5" t="n"/>
+      <c r="G96" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" ht="18.75" customHeight="1">
-      <c r="A97" s="2" t="inlineStr">
+      <c r="A97" s="5" t="inlineStr">
         <is>
           <t>Helena</t>
         </is>
       </c>
-      <c r="B97" s="2" t="inlineStr">
+      <c r="B97" s="5" t="inlineStr">
         <is>
           <t>Jabłońska</t>
         </is>
       </c>
-      <c r="C97" s="2" t="inlineStr">
+      <c r="C97" s="3" t="inlineStr">
         <is>
           <t>H. J.</t>
         </is>
       </c>
+      <c r="D97" s="2" t="n"/>
+      <c r="E97" s="2" t="n"/>
+      <c r="F97" s="5" t="n"/>
+      <c r="G97" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" ht="18.75" customHeight="1">
-      <c r="A98" s="2" t="inlineStr">
+      <c r="A98" s="5" t="inlineStr">
         <is>
           <t>Irena</t>
         </is>
       </c>
-      <c r="B98" s="2" t="inlineStr">
+      <c r="B98" s="5" t="inlineStr">
         <is>
           <t>Zielińska</t>
         </is>
       </c>
-      <c r="C98" s="2" t="inlineStr">
+      <c r="C98" s="3" t="inlineStr">
         <is>
           <t>I. Z.</t>
         </is>
       </c>
+      <c r="D98" s="2" t="n"/>
+      <c r="E98" s="2" t="n"/>
+      <c r="F98" s="5" t="n"/>
+      <c r="G98" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" ht="18.75" customHeight="1">
-      <c r="A99" s="2" t="inlineStr">
+      <c r="A99" s="5" t="inlineStr">
         <is>
           <t>Halina</t>
         </is>
       </c>
-      <c r="B99" s="2" t="inlineStr">
+      <c r="B99" s="5" t="inlineStr">
         <is>
           <t>Przybylska</t>
         </is>
       </c>
-      <c r="C99" s="2" t="inlineStr">
+      <c r="C99" s="3" t="inlineStr">
         <is>
           <t>H. P.</t>
         </is>
       </c>
+      <c r="D99" s="2" t="n"/>
+      <c r="E99" s="2" t="n"/>
+      <c r="F99" s="5" t="n"/>
+      <c r="G99" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" ht="18.75" customHeight="1">
-      <c r="A100" s="2" t="inlineStr">
+      <c r="A100" s="5" t="inlineStr">
         <is>
           <t>Izabela</t>
         </is>
       </c>
-      <c r="B100" s="2" t="inlineStr">
+      <c r="B100" s="5" t="inlineStr">
         <is>
           <t>Czarnecka</t>
         </is>
       </c>
-      <c r="C100" s="2" t="inlineStr">
+      <c r="C100" s="3" t="inlineStr">
         <is>
           <t>I. C.</t>
         </is>
       </c>
+      <c r="D100" s="2" t="n"/>
+      <c r="E100" s="2" t="n"/>
+      <c r="F100" s="5" t="n"/>
+      <c r="G100" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" ht="18.75" customHeight="1">
-      <c r="A101" s="2" t="inlineStr">
+      <c r="A101" s="5" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="B101" s="2" t="inlineStr">
+      <c r="B101" s="5" t="inlineStr">
         <is>
           <t>Chmielewski</t>
         </is>
       </c>
-      <c r="C101" s="2" t="inlineStr">
+      <c r="C101" s="3" t="inlineStr">
         <is>
           <t>P. C.</t>
         </is>
       </c>
+      <c r="D101" s="2" t="n"/>
+      <c r="E101" s="2" t="n"/>
+      <c r="F101" s="5" t="n"/>
+      <c r="G101" s="2" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="102" ht="18.75" customHeight="1">
-      <c r="A102" s="2" t="n"/>
-      <c r="B102" s="2" t="n"/>
-      <c r="C102" s="2" t="n"/>
+      <c r="A102" s="5" t="n"/>
+      <c r="B102" s="5" t="n"/>
+      <c r="C102" s="5" t="n"/>
+      <c r="D102" s="2" t="n"/>
+      <c r="E102" s="2" t="n"/>
+      <c r="F102" s="5" t="n"/>
+      <c r="G102" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>